<commit_message>
02/20: Enhancing framework for Contacts tab
</commit_message>
<xml_diff>
--- a/FreeCRMTestDataSheet.xlsx
+++ b/FreeCRMTestDataSheet.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Companies" sheetId="1" r:id="rId1"/>
+    <sheet name="Contacts" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Company</t>
   </si>
@@ -35,6 +36,51 @@
   </si>
   <si>
     <t>Active</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Dr.</t>
+  </si>
+  <si>
+    <t>Matt</t>
+  </si>
+  <si>
+    <t>Williams</t>
+  </si>
+  <si>
+    <t>Mediaocean Asia Pvt. Ltd.</t>
+  </si>
+  <si>
+    <t>Mr.</t>
+  </si>
+  <si>
+    <t>Mark</t>
+  </si>
+  <si>
+    <t>Keller</t>
+  </si>
+  <si>
+    <t>Cognizant Technology Solutions Pvt. Ltd.</t>
+  </si>
+  <si>
+    <t>Mrs.</t>
+  </si>
+  <si>
+    <t>Anshika</t>
+  </si>
+  <si>
+    <t>Khandelwal</t>
+  </si>
+  <si>
+    <t>Infosys Pvt. Ltd.</t>
   </si>
 </sst>
 </file>
@@ -391,7 +437,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -434,4 +480,81 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.90625" customWidth="1"/>
+    <col min="2" max="2" width="19.81640625" customWidth="1"/>
+    <col min="3" max="3" width="22.90625" customWidth="1"/>
+    <col min="4" max="4" width="40.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
02/25- Committing minor changes to fix test NG errors
</commit_message>
<xml_diff>
--- a/FreeCRMTestDataSheet.xlsx
+++ b/FreeCRMTestDataSheet.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="1"/>
@@ -10,12 +10,12 @@
     <sheet name="Companies" sheetId="1" r:id="rId1"/>
     <sheet name="Contacts" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Company</t>
   </si>
@@ -50,44 +50,53 @@
     <t>Dr.</t>
   </si>
   <si>
-    <t>Matt</t>
-  </si>
-  <si>
-    <t>Williams</t>
-  </si>
-  <si>
     <t>Mediaocean Asia Pvt. Ltd.</t>
   </si>
   <si>
     <t>Mr.</t>
   </si>
   <si>
-    <t>Mark</t>
-  </si>
-  <si>
-    <t>Keller</t>
-  </si>
-  <si>
     <t>Cognizant Technology Solutions Pvt. Ltd.</t>
   </si>
   <si>
     <t>Mrs.</t>
   </si>
   <si>
-    <t>Anshika</t>
-  </si>
-  <si>
-    <t>Khandelwal</t>
-  </si>
-  <si>
     <t>Infosys Pvt. Ltd.</t>
+  </si>
+  <si>
+    <t>Manpreet</t>
+  </si>
+  <si>
+    <t>Singh</t>
+  </si>
+  <si>
+    <t>Limestone Pvt. Ltd.</t>
+  </si>
+  <si>
+    <t>Gunit</t>
+  </si>
+  <si>
+    <t>Thapar</t>
+  </si>
+  <si>
+    <t>Asheen</t>
+  </si>
+  <si>
+    <t>Antony</t>
+  </si>
+  <si>
+    <t>Rahul</t>
+  </si>
+  <si>
+    <t>Varma</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,7 +200,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -223,10 +232,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -258,7 +266,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -434,14 +441,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="25.81640625" customWidth="1"/>
     <col min="2" max="2" width="20.453125" customWidth="1"/>
@@ -449,7 +456,7 @@
     <col min="4" max="4" width="19.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -463,7 +470,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -483,14 +490,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="15.90625" customWidth="1"/>
     <col min="2" max="2" width="19.81640625" customWidth="1"/>
@@ -498,7 +505,7 @@
     <col min="4" max="4" width="40.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -512,46 +519,60 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
         <v>18</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
02/27: Enhancing extent reports to capture screen shot on failure (ContactsTest)
</commit_message>
<xml_diff>
--- a/FreeCRMTestDataSheet.xlsx
+++ b/FreeCRMTestDataSheet.xlsx
@@ -59,9 +59,6 @@
     <t>Cognizant Technology Solutions Pvt. Ltd.</t>
   </si>
   <si>
-    <t>Mrs.</t>
-  </si>
-  <si>
     <t>Infosys Pvt. Ltd.</t>
   </si>
   <si>
@@ -90,6 +87,9 @@
   </si>
   <si>
     <t>Varma</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -494,7 +494,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -524,10 +524,10 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
         <v>19</v>
-      </c>
-      <c r="C2" t="s">
-        <v>20</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
@@ -538,10 +538,10 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
         <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>22</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
@@ -549,16 +549,16 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
         <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -566,13 +566,13 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
         <v>23</v>
       </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
03/06- Updating config.properties to contains file paths
</commit_message>
<xml_diff>
--- a/FreeCRMTestDataSheet.xlsx
+++ b/FreeCRMTestDataSheet.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>Company</t>
   </si>
@@ -87,9 +87,6 @@
   </si>
   <si>
     <t>Varma</t>
-  </si>
-  <si>
-    <t>test</t>
   </si>
 </sst>
 </file>
@@ -494,7 +491,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -549,7 +546,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>

</xml_diff>